<commit_message>
adjusting state counts spreadsheet
</commit_message>
<xml_diff>
--- a/DesignNotes/Data Model and SQL/Analyses/state counts.xlsx
+++ b/DesignNotes/Data Model and SQL/Analyses/state counts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710"/>
   </bookViews>
@@ -47,6 +47,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,14 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -123,26 +125,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="86">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -405,6 +430,54 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.59999389629810485"/>
@@ -415,6 +488,38 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
@@ -423,6 +528,38 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
@@ -431,20 +568,44 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.39997558519241921"/>
@@ -479,6 +640,38 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
@@ -487,6 +680,22 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
@@ -494,7 +703,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
@@ -502,306 +710,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1335,8 +1244,8 @@
   <dataFields count="1">
     <dataField name="Sum of State Count" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="80">
-    <format dxfId="95">
+  <formats count="82">
+    <format dxfId="85">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1348,7 +1257,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="84">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1360,7 +1269,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="83">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1372,7 +1281,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="82">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1384,7 +1293,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="81">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -1396,7 +1305,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="80">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -1405,6 +1314,30 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="79">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="78">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="77">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
@@ -1412,64 +1345,244 @@
             <x v="11"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="75">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="10"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="72">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="11"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="9"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="63">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="10"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="11"/>
+    <format dxfId="57">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="2"/>
@@ -1477,23 +1590,47 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="8"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="55">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
+    <format dxfId="53">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
@@ -1501,11 +1638,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="10"/>
+    <format dxfId="52">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="2"/>
@@ -1513,11 +1650,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="11"/>
+    <format dxfId="51">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="3"/>
@@ -1525,307 +1662,79 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="50">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="49">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="48">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="47">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="46">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="7"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="66">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="65">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="64">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="10"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="63">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="11"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
             <x v="4"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="61">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="60">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="59">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="58">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="10"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="57">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="56">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="55">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="54">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="53">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="52">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="51">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="50">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="47">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="46">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
     <format dxfId="44">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="43">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="42">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="4">
@@ -1837,43 +1746,211 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="43">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="42">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="41">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="39">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="33">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
             <x v="8"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
@@ -1881,11 +1958,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="10"/>
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="2"/>
@@ -1893,11 +1970,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="11"/>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="7"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="3"/>
@@ -1905,23 +1982,95 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
             <x v="7"/>
           </reference>
           <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="3"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
@@ -1929,11 +2078,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="2"/>
@@ -1941,11 +2090,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="10"/>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="4"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="3"/>
@@ -1953,11 +2102,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="11"/>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="5"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="4"/>
@@ -1965,303 +2114,78 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
             <x v="0"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
             <x v="1"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
             <x v="2"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
             <x v="3"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="9"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
             <x v="4"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
+          <reference field="1" count="1" selected="0">
             <x v="4"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="18">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="14">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
-          <reference field="0" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
+          <reference field="0" count="0"/>
+          <reference field="1" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
     <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
+      <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
@@ -2627,13 +2551,13 @@
   <dimension ref="A3:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="16" style="6" customWidth="1"/>
+    <col min="2" max="6" width="16" style="5" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2641,7 +2565,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2649,19 +2573,19 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>4</v>
       </c>
       <c r="G4" t="s">
@@ -2672,22 +2596,22 @@
       <c r="A5" s="2">
         <v>12</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>558696743</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>127891832</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>6254362</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="8">
         <v>164960</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <v>531</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="13">
         <v>693008428</v>
       </c>
     </row>
@@ -2695,22 +2619,22 @@
       <c r="A6" s="2">
         <v>11</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="9">
         <v>581379204</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>212768805</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>20174891</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <v>1228616</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <v>19616</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="13">
         <v>815571132</v>
       </c>
     </row>
@@ -2718,22 +2642,22 @@
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>430688976</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="9">
         <v>237780102</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>40855588</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>4782029</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="8">
         <v>219696</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="13">
         <v>714326391</v>
       </c>
     </row>
@@ -2741,22 +2665,22 @@
       <c r="A8" s="2">
         <v>9</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>231416681</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>185457162</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>55007415</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>11378264</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="8">
         <v>1193504</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="13">
         <v>484453026</v>
       </c>
     </row>
@@ -2764,22 +2688,22 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>91133282</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>103673970</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>51283334</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>18015812</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>3744239</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="13">
         <v>267850637</v>
       </c>
     </row>
@@ -2787,22 +2711,22 @@
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>26377978</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>42302857</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>34139846</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>19834499</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>7271709</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="13">
         <v>129926889</v>
       </c>
     </row>
@@ -2810,22 +2734,22 @@
       <c r="A11" s="2">
         <v>6</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="7">
         <v>5582402</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>12738329</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>16564082</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>15427621</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="9">
         <v>9093822</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="14">
         <v>59406256</v>
       </c>
     </row>
@@ -2833,22 +2757,22 @@
       <c r="A12" s="2">
         <v>5</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>850768</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>2838221</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>5898264</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>8496152</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>7585481</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="13">
         <v>25668886</v>
       </c>
     </row>
@@ -2856,22 +2780,22 @@
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>90633</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>463472</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>1529878</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>3318478</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>4394554</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="13">
         <v>9797015</v>
       </c>
     </row>
@@ -2879,22 +2803,22 @@
       <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="12">
         <v>6388</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>53900</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>283330</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>921239</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>1812366</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="13">
         <v>3077223</v>
       </c>
     </row>
@@ -2902,22 +2826,22 @@
       <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <v>267</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="12">
         <v>4204</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>36203</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>180076</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>532824</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="13">
         <v>753574</v>
       </c>
     </row>
@@ -2925,22 +2849,22 @@
       <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="12">
         <v>5</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>196</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="12">
         <v>3056</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>24818</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>115368</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="13">
         <v>143443</v>
       </c>
     </row>
@@ -2948,19 +2872,19 @@
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>1926223327</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>925973050</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>232030249</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>83772564</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>35983710</v>
       </c>
       <c r="G17" s="3">

</xml_diff>